<commit_message>
back end teszt done
</commit_message>
<xml_diff>
--- a/diagrams/tesztadatok.xlsx
+++ b/diagrams/tesztadatok.xlsx
@@ -28,17 +28,20 @@
   <connection id="1" name="aston_martin_vantage_4.7l_sp-10_sportshift-9257234" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="D:\bes\src\test\aston_martin_vantage_4.7l_sp-10_sportshift-9257234.xml" htmlTables="1"/>
   </connection>
-  <connection id="2" name="values_aston_martin_vantage_4.7l_sp-10_sportshift-9257234" type="4" refreshedVersion="0" background="1">
+  <connection id="2" name="audi_a3_limousine_1.4_tfsi_attraction_mo.i-2600km_s-line-9671311" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="D:\bes\src\test\audi_a3_limousine_1.4_tfsi_attraction_mo.i-2600km_s-line-9671311.xml" htmlTables="1"/>
+  </connection>
+  <connection id="3" name="values_aston_martin_vantage_4.7l_sp-10_sportshift-9257234" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="D:\bes\output\values_aston_martin_vantage_4.7l_sp-10_sportshift-9257234.xml" htmlTables="1"/>
   </connection>
-  <connection id="3" name="values_aston_martin_vantage_4.7l_sp-10_sportshift-92572341" type="4" refreshedVersion="0" background="1">
+  <connection id="4" name="values_aston_martin_vantage_4.7l_sp-10_sportshift-92572341" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="D:\bes\output\values_aston_martin_vantage_4.7l_sp-10_sportshift-9257234.xml" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Mass</t>
   </si>
@@ -92,6 +95,30 @@
   </si>
   <si>
     <t>Worth</t>
+  </si>
+  <si>
+    <t>92 kW, 125 LE</t>
+  </si>
+  <si>
+    <t>2 600 km</t>
+  </si>
+  <si>
+    <t>1 215 kg</t>
+  </si>
+  <si>
+    <t>6.599.000 Ft</t>
+  </si>
+  <si>
+    <t>Megkímélt</t>
+  </si>
+  <si>
+    <t>2015/3</t>
+  </si>
+  <si>
+    <t>Csomagtartó</t>
+  </si>
+  <si>
+    <t>Tömeg</t>
   </si>
 </sst>
 </file>
@@ -115,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,13 +150,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -331,14 +371,64 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema4" Namespace="http://schemas.microsoft.com/powershell/2004/04">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:ns0="http://schemas.microsoft.com/powershell/2004/04" xmlns="" targetNamespace="http://schemas.microsoft.com/powershell/2004/04">
+      <xsd:element nillable="true" name="Objs">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" nillable="true" name="Obj" form="qualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" name="TN" form="qualified">
+                    <xsd:complexType>
+                      <xsd:sequence minOccurs="0">
+                        <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" type="xsd:string" name="T" form="qualified"/>
+                      </xsd:sequence>
+                      <xsd:attribute name="RefId" form="unqualified" type="xsd:integer"/>
+                    </xsd:complexType>
+                  </xsd:element>
+                  <xsd:element minOccurs="0" nillable="true" name="DCT" form="qualified">
+                    <xsd:complexType>
+                      <xsd:sequence minOccurs="0">
+                        <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="En" form="qualified">
+                          <xsd:complexType>
+                            <xsd:sequence minOccurs="0">
+                              <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="S" form="qualified">
+                                <xsd:complexType>
+                                  <xsd:simpleContent>
+                                    <xsd:extension base="xsd:string">
+                                      <xsd:attribute name="N" form="unqualified" type="xsd:string"/>
+                                    </xsd:extension>
+                                  </xsd:simpleContent>
+                                </xsd:complexType>
+                              </xsd:element>
+                            </xsd:sequence>
+                          </xsd:complexType>
+                        </xsd:element>
+                      </xsd:sequence>
+                    </xsd:complexType>
+                  </xsd:element>
+                </xsd:sequence>
+                <xsd:attribute name="RefId" form="unqualified" type="xsd:integer"/>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+          <xsd:attribute name="Version" form="unqualified" type="xsd:string"/>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="1" Name="Objs_megfeleltetés" RootElement="Objs" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="2" Name="Objs_megfeleltetés1" RootElement="Objs" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="3" Name="Objs_megfeleltetés2" RootElement="Objs" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  </Map>
+  <Map ID="4" Name="Objs_megfeleltetés3" RootElement="Objs" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
@@ -606,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B15"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,118 +707,416 @@
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B11" s="1">
         <v>-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B12" s="1">
         <v>-13.333333333333334</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="D12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B13" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B14" s="1">
         <v>-1.7078</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B16" s="1">
         <v>22.857142857142858</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1">
-        <f>SUM(B8:B14)</f>
+      <c r="B18" s="1">
+        <f>SUM(B11:B17)</f>
         <v>14.816009523809521</v>
       </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>